<commit_message>
problem witn counter calcuclation
</commit_message>
<xml_diff>
--- a/Template_apl_cycles.xlsx
+++ b/Template_apl_cycles.xlsx
@@ -1244,7 +1244,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="79" t="n">
-        <v>89</v>
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="9" s="89" spans="1:9" thickBot="1">
@@ -1658,7 +1658,7 @@
         <v>18</v>
       </c>
       <c r="F44" s="75" t="n">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="G44" s="90" t="n"/>
       <c r="H44" s="90" t="n"/>

</xml_diff>

<commit_message>
add test exe file - not work
</commit_message>
<xml_diff>
--- a/Template_apl_cycles.xlsx
+++ b/Template_apl_cycles.xlsx
@@ -1244,7 +1244,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="79" t="n">
-        <v>89</v>
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="9" s="89" spans="1:9" thickBot="1">
@@ -1658,7 +1658,7 @@
         <v>18</v>
       </c>
       <c r="F44" s="75" t="n">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="G44" s="90" t="n"/>
       <c r="H44" s="90" t="n"/>

</xml_diff>

<commit_message>
check same action with 1 row
</commit_message>
<xml_diff>
--- a/Template_apl_cycles.xlsx
+++ b/Template_apl_cycles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="11955" windowWidth="27495" xWindow="630" yWindow="600"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="print1" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
   <definedNames>
     <definedName localSheetId="0" name="_xlnm.Print_Area">print1!$A$1:$J$44</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="35" t="n">
-        <v>80002132</v>
+        <v>89</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="9" s="27" spans="1:9" thickBot="1">
@@ -898,7 +898,9 @@
       <c r="B11" s="30" t="n"/>
       <c r="C11" s="30" t="n"/>
       <c r="D11" s="30" t="n"/>
-      <c r="E11" s="31" t="n"/>
+      <c r="E11" s="31" t="n">
+        <v>4001</v>
+      </c>
       <c r="F11" s="30" t="n"/>
       <c r="G11" s="30" t="n"/>
       <c r="H11" s="30" t="n"/>
@@ -1265,7 +1267,7 @@
         <v>18</v>
       </c>
       <c r="F44" s="23" t="n">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="G44" s="28" t="n"/>
       <c r="H44" s="28" t="n"/>

</xml_diff>